<commit_message>
put upto ceiling into excel file
</commit_message>
<xml_diff>
--- a/code/cg_interia/aircraft_items.xlsx
+++ b/code/cg_interia/aircraft_items.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -46,23 +46,42 @@
     <t xml:space="preserve">H (m)</t>
   </si>
   <si>
-    <t xml:space="preserve">Seat Left 1350</t>
+    <t xml:space="preserve">Triple Seat (yellow)</t>
   </si>
   <si>
-    <t xml:space="preserve">Seat Left 1150</t>
+    <t xml:space="preserve">Double Seat (yellow)</t>
   </si>
   <si>
-    <t xml:space="preserve">Seat Right 1350</t>
+    <t xml:space="preserve">Toilet (front)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toilet (back)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kitchen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emergency Slides</t>
+  </si>
+  <si>
+    <t xml:space="preserve">?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lift Rafts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ceiling</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -84,6 +103,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -128,8 +153,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -150,15 +179,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB22" activeCellId="0" sqref="AB22"/>
+      <selection pane="topLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -192,7 +227,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>-7</v>
@@ -217,11 +252,11 @@
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="str">
         <f aca="false">A2</f>
-        <v>Seat Left 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B3" s="0" t="n">
         <f aca="false">B2</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C3" s="0" t="n">
         <f aca="false">C2-0.4</f>
@@ -251,11 +286,11 @@
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="str">
         <f aca="false">A3</f>
-        <v>Seat Left 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">B3</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C4" s="0" t="n">
         <f aca="false">C3-0.4</f>
@@ -285,11 +320,11 @@
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="str">
         <f aca="false">A4</f>
-        <v>Seat Left 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B5" s="0" t="n">
         <f aca="false">B4</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C5" s="0" t="n">
         <f aca="false">C4-0.4</f>
@@ -319,11 +354,11 @@
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="str">
         <f aca="false">A5</f>
-        <v>Seat Left 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B6" s="0" t="n">
         <f aca="false">B5</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C6" s="0" t="n">
         <f aca="false">C5-0.4</f>
@@ -353,11 +388,11 @@
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="str">
         <f aca="false">A6</f>
-        <v>Seat Left 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B7" s="0" t="n">
         <f aca="false">B6</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C7" s="0" t="n">
         <f aca="false">C6-0.4</f>
@@ -387,11 +422,11 @@
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="str">
         <f aca="false">A7</f>
-        <v>Seat Left 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B8" s="0" t="n">
         <f aca="false">B7</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C8" s="0" t="n">
         <f aca="false">C7-0.4</f>
@@ -421,11 +456,11 @@
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="str">
         <f aca="false">A8</f>
-        <v>Seat Left 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B9" s="0" t="n">
         <f aca="false">B8</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C9" s="0" t="n">
         <f aca="false">C8-0.4</f>
@@ -455,11 +490,11 @@
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="str">
         <f aca="false">A9</f>
-        <v>Seat Left 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B10" s="0" t="n">
         <f aca="false">B9</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C10" s="0" t="n">
         <f aca="false">C9-0.4</f>
@@ -489,11 +524,11 @@
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="str">
         <f aca="false">A10</f>
-        <v>Seat Left 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">B10</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C11" s="0" t="n">
         <f aca="false">C10-0.4</f>
@@ -523,11 +558,11 @@
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="str">
         <f aca="false">A11</f>
-        <v>Seat Left 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B12" s="0" t="n">
         <f aca="false">B11</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C12" s="0" t="n">
         <f aca="false">C11-0.4</f>
@@ -557,11 +592,11 @@
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="str">
         <f aca="false">A12</f>
-        <v>Seat Left 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B13" s="0" t="n">
         <f aca="false">B12</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C13" s="0" t="n">
         <f aca="false">C12-0.4</f>
@@ -591,11 +626,11 @@
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="str">
         <f aca="false">A13</f>
-        <v>Seat Left 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B14" s="0" t="n">
         <f aca="false">B13</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C14" s="0" t="n">
         <f aca="false">C13-0.4</f>
@@ -625,11 +660,11 @@
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="str">
         <f aca="false">A14</f>
-        <v>Seat Left 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B15" s="0" t="n">
         <f aca="false">B14</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C15" s="0" t="n">
         <f aca="false">C14-0.4</f>
@@ -659,11 +694,11 @@
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="str">
         <f aca="false">A15</f>
-        <v>Seat Left 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B16" s="0" t="n">
         <f aca="false">B15</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C16" s="0" t="n">
         <f aca="false">C15-0.4</f>
@@ -693,11 +728,11 @@
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="str">
         <f aca="false">A16</f>
-        <v>Seat Left 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B17" s="0" t="n">
         <f aca="false">B16</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C17" s="0" t="n">
         <f aca="false">C16-0.4</f>
@@ -727,11 +762,11 @@
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="str">
         <f aca="false">A17</f>
-        <v>Seat Left 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B18" s="0" t="n">
         <f aca="false">B17</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C18" s="0" t="n">
         <f aca="false">C17-0.4</f>
@@ -763,7 +798,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>27</v>
+        <v>36.6626</v>
       </c>
       <c r="C19" s="0" t="n">
         <f aca="false">C18-0.4</f>
@@ -789,12 +824,13 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>9</v>
+      <c r="A20" s="0" t="str">
+        <f aca="false">A19</f>
+        <v>Double Seat (yellow)</v>
       </c>
       <c r="B20" s="0" t="n">
         <f aca="false">B19</f>
-        <v>27</v>
+        <v>36.6626</v>
       </c>
       <c r="C20" s="0" t="n">
         <f aca="false">C19-0.4</f>
@@ -822,11 +858,12 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>10</v>
+      <c r="A21" s="0" t="str">
+        <f aca="false">A18</f>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>-7</v>
@@ -850,14 +887,14 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="str">
         <f aca="false">A21</f>
-        <v>Seat Right 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B22" s="0" t="n">
         <f aca="false">B21</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C22" s="0" t="n">
         <f aca="false">C21-0.4</f>
@@ -884,14 +921,14 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="str">
         <f aca="false">A22</f>
-        <v>Seat Right 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B23" s="0" t="n">
         <f aca="false">B22</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C23" s="0" t="n">
         <f aca="false">C22-0.4</f>
@@ -918,14 +955,14 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="str">
         <f aca="false">A23</f>
-        <v>Seat Right 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B24" s="0" t="n">
         <f aca="false">B23</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C24" s="0" t="n">
         <f aca="false">C23-0.4</f>
@@ -952,14 +989,14 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="str">
         <f aca="false">A24</f>
-        <v>Seat Right 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B25" s="0" t="n">
         <f aca="false">B24</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C25" s="0" t="n">
         <f aca="false">C24-0.4</f>
@@ -986,14 +1023,14 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="str">
         <f aca="false">A25</f>
-        <v>Seat Right 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B26" s="0" t="n">
         <f aca="false">B25</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C26" s="0" t="n">
         <f aca="false">C25-0.4</f>
@@ -1020,14 +1057,14 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="str">
         <f aca="false">A26</f>
-        <v>Seat Right 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B27" s="0" t="n">
         <f aca="false">B26</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C27" s="0" t="n">
         <f aca="false">C26-0.4</f>
@@ -1054,14 +1091,14 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="str">
         <f aca="false">A27</f>
-        <v>Seat Right 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B28" s="0" t="n">
         <f aca="false">B27</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C28" s="0" t="n">
         <f aca="false">C27-0.4</f>
@@ -1088,14 +1125,14 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="str">
         <f aca="false">A28</f>
-        <v>Seat Right 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B29" s="0" t="n">
         <f aca="false">B28</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C29" s="0" t="n">
         <f aca="false">C28-0.4</f>
@@ -1122,14 +1159,14 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="str">
         <f aca="false">A29</f>
-        <v>Seat Right 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B30" s="0" t="n">
         <f aca="false">B29</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C30" s="0" t="n">
         <f aca="false">C29-0.4</f>
@@ -1156,14 +1193,14 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="str">
         <f aca="false">A30</f>
-        <v>Seat Right 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B31" s="0" t="n">
         <f aca="false">B30</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C31" s="0" t="n">
         <f aca="false">C30-0.4</f>
@@ -1190,14 +1227,14 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="str">
         <f aca="false">A31</f>
-        <v>Seat Right 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B32" s="0" t="n">
         <f aca="false">B31</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C32" s="0" t="n">
         <f aca="false">C31-0.4</f>
@@ -1224,14 +1261,14 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="str">
         <f aca="false">A32</f>
-        <v>Seat Right 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B33" s="0" t="n">
         <f aca="false">B32</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C33" s="0" t="n">
         <f aca="false">C32-0.4</f>
@@ -1258,14 +1295,14 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="str">
         <f aca="false">A33</f>
-        <v>Seat Right 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B34" s="0" t="n">
         <f aca="false">B33</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C34" s="0" t="n">
         <f aca="false">C33-0.4</f>
@@ -1292,14 +1329,14 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="str">
         <f aca="false">A34</f>
-        <v>Seat Right 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B35" s="0" t="n">
         <f aca="false">B34</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C35" s="0" t="n">
         <f aca="false">C34-0.4</f>
@@ -1326,14 +1363,14 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="str">
         <f aca="false">A35</f>
-        <v>Seat Right 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B36" s="0" t="n">
         <f aca="false">B35</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C36" s="0" t="n">
         <f aca="false">C35-0.4</f>
@@ -1360,14 +1397,14 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="str">
         <f aca="false">A36</f>
-        <v>Seat Right 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B37" s="0" t="n">
         <f aca="false">B36</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C37" s="0" t="n">
         <f aca="false">C36-0.4</f>
@@ -1394,14 +1431,14 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="str">
         <f aca="false">A37</f>
-        <v>Seat Right 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B38" s="0" t="n">
         <f aca="false">B37</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C38" s="0" t="n">
         <f aca="false">C37-0.4</f>
@@ -1428,14 +1465,14 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="str">
         <f aca="false">A38</f>
-        <v>Seat Right 1350</v>
+        <v>Triple Seat (yellow)</v>
       </c>
       <c r="B39" s="0" t="n">
         <f aca="false">B38</f>
-        <v>44</v>
+        <v>56.5191</v>
       </c>
       <c r="C39" s="0" t="n">
         <f aca="false">C38-0.4</f>
@@ -1462,6 +1499,187 @@
         <v>1.3</v>
       </c>
     </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>-6</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>-1.11</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>-1.44</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G40" s="0" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="H40" s="0" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>-26</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>-1.11</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>-1.44</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <f aca="false">F40</f>
+        <v>1</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <f aca="false">G40</f>
+        <v>1.1</v>
+      </c>
+      <c r="H41" s="0" t="n">
+        <f aca="false">H40</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>138</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>-27.75</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>-1.195</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G42" s="0" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="H42" s="0" t="n">
+        <v>2.01</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F43" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G43" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H43" s="0" t="n">
+        <v>1.14</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F44" s="1" t="n">
+        <f aca="false">F43</f>
+        <v>0.5</v>
+      </c>
+      <c r="G44" s="1" t="n">
+        <f aca="false">G43</f>
+        <v>0.1</v>
+      </c>
+      <c r="H44" s="1" t="n">
+        <f aca="false">H43</f>
+        <v>1.14</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>600</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>-15.6</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>-2.32</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <v>20.2</v>
+      </c>
+      <c r="G45" s="0" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="H45" s="0" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>